<commit_message>
setting maatschappij column to edit (set x) in
</commit_message>
<xml_diff>
--- a/static/new.xlsx
+++ b/static/new.xlsx
@@ -4,7 +4,6 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="6020" sheetId="1" r:id="rId1"/>
-    <sheet name="06020" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -481,17 +480,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
prepare excel controller for modifying the file
</commit_message>
<xml_diff>
--- a/static/new.xlsx
+++ b/static/new.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="6020" sheetId="1" r:id="rId1"/>
+    <sheet name="06020" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -480,4 +481,38 @@
     <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Omschrijving</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Inhoud</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Weergave</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Uitlijnen</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Regel verwijderen</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Regel template</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
increase range !ref and set maatschappij column to new maatschappij
</commit_message>
<xml_diff>
--- a/static/new.xlsx
+++ b/static/new.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -402,6 +402,9 @@
       <c r="G1" t="str">
         <v>P302</v>
       </c>
+      <c r="H1" t="str">
+        <v>P368</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -410,6 +413,9 @@
       <c r="B2">
         <v>10694</v>
       </c>
+      <c r="H2" t="str">
+        <v>x</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -449,7 +455,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
converted internals to 0-indexed numbers for clarity
</commit_message>
<xml_diff>
--- a/static/new.xlsx
+++ b/static/new.xlsx
@@ -402,19 +402,13 @@
       <c r="G1" t="str">
         <v>P302</v>
       </c>
-      <c r="H1" t="str">
-        <v>P368</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Gezinssamenstelling</v>
+        <v>x</v>
       </c>
       <c r="B2">
         <v>10694</v>
-      </c>
-      <c r="H2" t="str">
-        <v>x</v>
       </c>
     </row>
     <row r="3">
@@ -449,13 +443,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Eigen risico</v>
+        <v>x</v>
       </c>
       <c r="B6" t="str">
         <v>€ 10043  10044</v>
-      </c>
-      <c r="H6" t="str">
-        <v>x</v>
       </c>
     </row>
     <row r="7">
@@ -482,13 +473,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>n/a</v>
+        <v>x</v>
       </c>
       <c r="B9" t="str">
         <v>10631 10632 10630          10633</v>
-      </c>
-      <c r="H9" t="str">
-        <v>x</v>
       </c>
     </row>
     <row r="10">
@@ -533,6 +521,11 @@
       </c>
       <c r="E13" t="str">
         <v>verwijderen</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="str">
+        <v>asd</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
setting maatschappij works again, forgot to increase c
</commit_message>
<xml_diff>
--- a/static/new.xlsx
+++ b/static/new.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -405,10 +405,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>x</v>
+        <v>Gezinssamenstelling</v>
       </c>
       <c r="B2">
         <v>10694</v>
+      </c>
+      <c r="H2" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="3">
@@ -443,10 +446,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>x</v>
+        <v>Eigen risico</v>
       </c>
       <c r="B6" t="str">
         <v>€ 10043  10044</v>
+      </c>
+      <c r="H6" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="7">
@@ -473,10 +479,13 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>x</v>
+        <v>n/a</v>
       </c>
       <c r="B9" t="str">
         <v>10631 10632 10630          10633</v>
+      </c>
+      <c r="H9" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="10">
@@ -523,50 +532,10 @@
         <v>verwijderen</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="str">
-        <v>asd</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="str">
-        <v>asd</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>